<commit_message>
Refactor game settings and card properties for improved balance and gameplay
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Table 1</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
   <si>
     <t>Пшеница</t>
@@ -1341,7 +1344,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1349,8 +1352,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1363,6 +1366,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" ht="28.2" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -1386,16 +1390,19 @@
       <c r="G2" t="s" s="3">
         <v>7</v>
       </c>
+      <c r="H2" t="s" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" ht="60.2" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
@@ -1404,21 +1411,24 @@
         <v>1</v>
       </c>
       <c r="F3" t="s" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s" s="6">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="7">
+        <v>90</v>
       </c>
     </row>
     <row r="4" ht="60" customHeight="1">
       <c r="A4" t="s" s="8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s" s="10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="11">
         <v>3</v>
@@ -1427,21 +1437,24 @@
         <v>3</v>
       </c>
       <c r="F4" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s" s="10">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="H4" s="11">
+        <v>50</v>
       </c>
     </row>
     <row r="5" ht="60" customHeight="1">
       <c r="A5" t="s" s="8">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="11">
         <v>5</v>
@@ -1450,21 +1463,24 @@
         <v>2</v>
       </c>
       <c r="F5" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s" s="10">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="H5" s="11">
+        <v>50</v>
       </c>
     </row>
     <row r="6" ht="60" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s" s="9">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s" s="10">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="11">
         <v>8</v>
@@ -1473,21 +1489,24 @@
         <v>0</v>
       </c>
       <c r="F6" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s" s="10">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="H6" s="11">
+        <v>10</v>
       </c>
     </row>
     <row r="7" ht="60" customHeight="1">
       <c r="A7" t="s" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s" s="10">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="11">
         <v>5</v>
@@ -1496,21 +1515,24 @@
         <v>0</v>
       </c>
       <c r="F7" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s" s="10">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="H7" s="11">
+        <v>70</v>
       </c>
     </row>
     <row r="8" ht="60" customHeight="1">
       <c r="A8" t="s" s="8">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s" s="10">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="11">
         <v>7</v>
@@ -1519,15 +1541,18 @@
         <v>4</v>
       </c>
       <c r="F8" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s" s="10">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="H8" s="11">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Add narrative property to Card and update related loading and display logic
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>Table 1</t>
   </si>
@@ -40,46 +40,283 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Пшеница</t>
+    <t>Narrative</t>
+  </si>
+  <si>
+    <t>Пенсия пришла!</t>
   </si>
   <si>
     <t>Blue</t>
   </si>
   <si>
+    <t>GETALL 2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>pensia.jpg</t>
+  </si>
+  <si>
+    <t>Бабушки довольны</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>+2 монеты всем</t>
+  </si>
+  <si>
+    <t>Налоговые каникулы</t>
+  </si>
+  <si>
+    <t>GETALL 3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>new_year.png</t>
+  </si>
+  <si>
+    <t>С Новай годай!</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>+3 монеты всем</t>
+  </si>
+  <si>
+    <t>Фестиваль еды</t>
+  </si>
+  <si>
     <t>GETALL 1</t>
   </si>
   <si>
-    <t>RelaxerR - blured.png</t>
-  </si>
-  <si>
-    <t>Урожайный год для всех поселенцев!</t>
-  </si>
-  <si>
-    <t>Лесопилка</t>
+    <t>food.jpg</t>
+  </si>
+  <si>
+    <t>Шаурма за счёт мэра</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>+1 монета всем</t>
+  </si>
+  <si>
+    <t>Премия от спонсора</t>
+  </si>
+  <si>
+    <t>GETALL 4</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>primia.jpg</t>
+  </si>
+  <si>
+    <t>Щедрый олигарх</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>+4 монеты всем</t>
+  </si>
+  <si>
+    <t>Стипендия</t>
+  </si>
+  <si>
+    <t>GETALL 5</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>stipendia.jpg</t>
+  </si>
+  <si>
+    <t>Ура стипа!</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>+5 монет всем</t>
+  </si>
+  <si>
+    <t>Агрессивный коллектор</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>STEAL_MONEY ALL 3</t>
+  </si>
+  <si>
+    <t>collector.jpg</t>
+  </si>
+  <si>
+    <t>Деньги есть?</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>Крадет 3 монеты у всех</t>
+  </si>
+  <si>
+    <t>Проверка пожарной</t>
+  </si>
+  <si>
+    <t>STEAL_MONEY ALL 2</t>
+  </si>
+  <si>
+    <t>pojarniy.jpg</t>
+  </si>
+  <si>
+    <t>Есть огнетушитель?</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>Крадет 2 монеты у всех</t>
+  </si>
+  <si>
+    <t>Рэкетир на районе</t>
+  </si>
+  <si>
+    <t>STEAL_MONEY RANDOM 5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>thief.jpg</t>
+  </si>
+  <si>
+    <t>Вор в законе</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Крадет 5 монет у случайного</t>
+  </si>
+  <si>
+    <t>Коррупционный скандал</t>
+  </si>
+  <si>
+    <t>STEAL_MONEY ALL 4</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>no_money.png</t>
+  </si>
+  <si>
+    <t>Чиновники нашли способ пополнить казну.</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Крадет 4 монеты у всех</t>
+  </si>
+  <si>
+    <t>Внезапный акциз</t>
+  </si>
+  <si>
+    <t>STEAL_MONEY ALL 6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>stonks.jpg</t>
+  </si>
+  <si>
+    <t>Утильсбор</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Крадет 6 монет у всех</t>
+  </si>
+  <si>
+    <t>Золотая жила</t>
   </si>
   <si>
     <t>Gold</t>
   </si>
   <si>
-    <t>GET 3</t>
-  </si>
-  <si>
-    <t>Приносит дерево и стабильный доход.</t>
-  </si>
-  <si>
-    <t>Налог</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>STEAL_MONEY ALL 2</t>
-  </si>
-  <si>
-    <t>Собирает по 2 монеты с каждого соседа.</t>
-  </si>
-  <si>
-    <t>Вор</t>
+    <t>GET 10</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>gold.jpg</t>
+  </si>
+  <si>
+    <t>Нашли нефть под гаражом</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>+10 монет</t>
+  </si>
+  <si>
+    <t>Инвестор из Дубая</t>
+  </si>
+  <si>
+    <t>GET 8</t>
+  </si>
+  <si>
+    <t>sahnov.png</t>
+  </si>
+  <si>
+    <t>Вы были приглашены в студию</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>+8 монет</t>
+  </si>
+  <si>
+    <t>Лотерейный билет</t>
+  </si>
+  <si>
+    <t>GET 15</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>casino.jpg</t>
+  </si>
+  <si>
+    <t>Джекпот!</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>+15 монет</t>
+  </si>
+  <si>
+    <t>Рейдерский захват</t>
   </si>
   <si>
     <t>Purple</t>
@@ -88,25 +325,16 @@
     <t>STEAL_CARD RANDOM</t>
   </si>
   <si>
-    <t>Позволяет забрать чужое предприятие.</t>
-  </si>
-  <si>
-    <t>Рынок</t>
-  </si>
-  <si>
-    <t>GETBY Blue 2</t>
-  </si>
-  <si>
-    <t>Бонус +2 за каждое ваше синее поле.</t>
-  </si>
-  <si>
-    <t>Трактир</t>
-  </si>
-  <si>
-    <t>STEAL_MONEY ALL 4</t>
-  </si>
-  <si>
-    <t>Крупный куш за счет кошельков других.</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>raider.jpg</t>
+  </si>
+  <si>
+    <t>На нас напали!</t>
+  </si>
+  <si>
+    <t>Крадет карту у случайного</t>
   </si>
 </sst>
 </file>
@@ -128,17 +356,30 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b val="1"/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -151,13 +392,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -166,7 +422,52 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -175,7 +476,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -184,73 +485,13 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
         <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -260,7 +501,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -270,31 +511,25 @@
     <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -314,8 +549,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1344,7 +1581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1352,8 +1589,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1367,8 +1604,9 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" ht="28.2" customHeight="1">
+    <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
@@ -1393,166 +1631,419 @@
       <c r="H2" t="s" s="3">
         <v>8</v>
       </c>
+      <c r="I2" t="s" s="3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" ht="60.2" customHeight="1">
+    <row r="3" ht="32.25" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" ht="32.05" customHeight="1">
+      <c r="A4" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s" s="8">
         <v>11</v>
       </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s" s="6">
+      <c r="C4" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s" s="9">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s" s="9">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" ht="32.05" customHeight="1">
+      <c r="A5" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s" s="9">
         <v>13</v>
       </c>
-      <c r="H3" s="7">
+      <c r="E5" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" ht="32.05" customHeight="1">
+      <c r="A6" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s" s="9">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s" s="9">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s" s="8">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="9">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s" s="9">
+        <v>42</v>
+      </c>
+      <c r="G7" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s" s="9">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" ht="32.05" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" ht="32.05" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s" s="9">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s" s="9">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s" s="9">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s" s="9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" ht="32.05" customHeight="1">
+      <c r="A10" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s" s="9">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s" s="9">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s" s="9">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s" s="9">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s" s="9">
+        <v>64</v>
+      </c>
+      <c r="I10" t="s" s="9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" ht="44.05" customHeight="1">
+      <c r="A11" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s" s="9">
+        <v>67</v>
+      </c>
+      <c r="D11" t="s" s="9">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s" s="9">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s" s="9">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s" s="9">
+        <v>71</v>
+      </c>
+      <c r="I11" t="s" s="9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" ht="32.05" customHeight="1">
+      <c r="A12" t="s" s="7">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s" s="9">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s" s="9">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s" s="9">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s" s="9">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s" s="9">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s" s="9">
+        <v>78</v>
+      </c>
+      <c r="I12" t="s" s="9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" ht="32.05" customHeight="1">
+      <c r="A13" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s" s="9">
+        <v>82</v>
+      </c>
+      <c r="D13" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s" s="9">
+        <v>83</v>
+      </c>
+      <c r="F13" t="s" s="9">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s" s="9">
+        <v>85</v>
+      </c>
+      <c r="H13" t="s" s="9">
+        <v>86</v>
+      </c>
+      <c r="I13" t="s" s="9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" ht="44.05" customHeight="1">
+      <c r="A14" t="s" s="7">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s" s="9">
+        <v>89</v>
+      </c>
+      <c r="D14" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s" s="9">
+        <v>75</v>
+      </c>
+      <c r="F14" t="s" s="9">
         <v>90</v>
       </c>
+      <c r="G14" t="s" s="9">
+        <v>91</v>
+      </c>
+      <c r="H14" t="s" s="9">
+        <v>92</v>
+      </c>
+      <c r="I14" t="s" s="9">
+        <v>93</v>
+      </c>
     </row>
-    <row r="4" ht="60" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>16</v>
-      </c>
-      <c r="D4" s="11">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="H4" s="11">
-        <v>50</v>
+    <row r="15" ht="32.05" customHeight="1">
+      <c r="A15" t="s" s="7">
+        <v>94</v>
+      </c>
+      <c r="B15" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s" s="9">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s" s="9">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s" s="9">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s" s="9">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s" s="9">
+        <v>98</v>
+      </c>
+      <c r="H15" t="s" s="9">
+        <v>99</v>
+      </c>
+      <c r="I15" t="s" s="9">
+        <v>100</v>
       </c>
     </row>
-    <row r="5" ht="60" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="D5" s="11">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11">
-        <v>2</v>
-      </c>
-      <c r="F5" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="H5" s="11">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" ht="60" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="D6" s="11">
-        <v>8</v>
-      </c>
-      <c r="E6" s="11">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="H6" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" ht="60" customHeight="1">
-      <c r="A7" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="D7" s="11">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s" s="10">
-        <v>28</v>
-      </c>
-      <c r="H7" s="11">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" ht="60" customHeight="1">
-      <c r="A8" t="s" s="8">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="D8" s="11">
-        <v>7</v>
-      </c>
-      <c r="E8" s="11">
-        <v>4</v>
-      </c>
-      <c r="F8" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="H8" s="11">
-        <v>40</v>
+    <row r="16" ht="32.05" customHeight="1">
+      <c r="A16" t="s" s="7">
+        <v>101</v>
+      </c>
+      <c r="B16" t="s" s="8">
+        <v>102</v>
+      </c>
+      <c r="C16" t="s" s="9">
+        <v>103</v>
+      </c>
+      <c r="D16" t="s" s="9">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s" s="9">
+        <v>104</v>
+      </c>
+      <c r="F16" t="s" s="9">
+        <v>105</v>
+      </c>
+      <c r="G16" t="s" s="9">
+        <v>106</v>
+      </c>
+      <c r="H16" t="s" s="9">
+        <v>96</v>
+      </c>
+      <c r="I16" t="s" s="9">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Refactor 21 02 26 (#3)
* Рефактор моделей

* Refactor logic

* refactor html,js,css
</commit_message>
<xml_diff>
--- a/Cards.xlsx
+++ b/Cards.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -52,6 +49,12 @@
     <t>GETALL 2</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>pensia.jpg</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t>GETALL 3</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>new_year.png</t>
   </si>
   <si>
@@ -106,6 +112,9 @@
     <t>GETALL 4</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>primia.jpg</t>
   </si>
   <si>
@@ -124,6 +133,9 @@
     <t>GETALL 5</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>stipendia.jpg</t>
   </si>
   <si>
@@ -181,6 +193,9 @@
     <t>STEAL_MONEY RANDOM 5</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>thief.jpg</t>
   </si>
   <si>
@@ -199,6 +214,9 @@
     <t>STEAL_MONEY ALL 4</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>no_money.png</t>
   </si>
   <si>
@@ -217,6 +235,9 @@
     <t>STEAL_MONEY ALL 6</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>stonks.jpg</t>
   </si>
   <si>
@@ -238,6 +259,9 @@
     <t>GET 10</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>gold.jpg</t>
   </si>
   <si>
@@ -274,6 +298,9 @@
     <t>GET 15</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>casino.jpg</t>
   </si>
   <si>
@@ -295,40 +322,16 @@
     <t>STEAL_CARD RANDOM</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>raider.jpg</t>
   </si>
   <si>
     <t>На нас напали!</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>Крадет карту у случайного</t>
-  </si>
-  <si>
-    <t>Корм для собак</t>
-  </si>
-  <si>
-    <t>dogs.png</t>
-  </si>
-  <si>
-    <t>Корм для всех</t>
-  </si>
-  <si>
-    <t>Дипломат</t>
-  </si>
-  <si>
-    <t>GET 2</t>
-  </si>
-  <si>
-    <t>diplomat.png</t>
-  </si>
-  <si>
-    <t>Договоримся?</t>
-  </si>
-  <si>
-    <t>+8 монеты</t>
   </si>
 </sst>
 </file>
@@ -495,15 +498,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -517,9 +517,6 @@
     <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -527,12 +524,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1584,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:I18"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1596,516 +1587,442 @@
     <col min="10" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
+    <row r="2" ht="32.25" customHeight="1">
       <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s" s="3">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s" s="3">
         <v>9</v>
       </c>
+      <c r="B2" t="s" s="4">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s" s="5">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s" s="5">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" ht="32.25" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" ht="32.05" customHeight="1">
+      <c r="A3" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s" s="7">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="6">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s" s="6">
+      <c r="C3" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s" s="8">
         <v>13</v>
       </c>
-      <c r="G3" t="s" s="6">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="I3" t="s" s="6">
-        <v>16</v>
+      <c r="E3" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s" s="8">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s" s="8">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s" s="8">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s" s="8">
+        <v>24</v>
       </c>
     </row>
     <row r="4" ht="32.05" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="D4" s="11">
-        <v>2</v>
-      </c>
-      <c r="E4" s="11">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s" s="10">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s" s="10">
-        <v>22</v>
+      <c r="A4" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s" s="8">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s" s="8">
+        <v>30</v>
       </c>
     </row>
     <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s" s="10">
-        <v>27</v>
-      </c>
-      <c r="I5" t="s" s="10">
-        <v>28</v>
+      <c r="A5" t="s" s="6">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="H5" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s" s="8">
+        <v>37</v>
       </c>
     </row>
-    <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" t="s" s="8">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s" s="10">
-        <v>30</v>
-      </c>
-      <c r="D6" s="11">
-        <v>3</v>
-      </c>
-      <c r="E6" s="11">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s" s="10">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s" s="10">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s" s="10">
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="6">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s" s="7">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="I6" t="s" s="10">
-        <v>34</v>
+      <c r="E6" t="s" s="8">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s" s="8">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s" s="8">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s" s="8">
+        <v>44</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="10">
-        <v>36</v>
-      </c>
-      <c r="D7" s="11">
-        <v>4</v>
-      </c>
-      <c r="E7" s="11">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s" s="10">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s" s="10">
-        <v>38</v>
-      </c>
-      <c r="H7" t="s" s="10">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s" s="10">
+    <row r="7" ht="32.05" customHeight="1">
+      <c r="A7" t="s" s="6">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s" s="8">
         <v>40</v>
+      </c>
+      <c r="E7" t="s" s="8">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s" s="8">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s" s="8">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s" s="8">
+        <v>51</v>
       </c>
     </row>
     <row r="8" ht="32.05" customHeight="1">
-      <c r="A8" t="s" s="8">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="D8" s="11">
-        <v>5</v>
-      </c>
-      <c r="E8" s="11">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s" s="10">
-        <v>44</v>
-      </c>
-      <c r="G8" t="s" s="10">
-        <v>45</v>
-      </c>
-      <c r="H8" t="s" s="10">
+      <c r="A8" t="s" s="6">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s" s="7">
         <v>46</v>
       </c>
-      <c r="I8" t="s" s="10">
-        <v>47</v>
+      <c r="C8" t="s" s="8">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s" s="8">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s" s="8">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s" s="8">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s" s="8">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s" s="8">
+        <v>57</v>
       </c>
     </row>
     <row r="9" ht="32.05" customHeight="1">
-      <c r="A9" t="s" s="8">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s" s="10">
-        <v>49</v>
-      </c>
-      <c r="D9" s="11">
-        <v>4</v>
-      </c>
-      <c r="E9" s="11">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s" s="10">
-        <v>50</v>
-      </c>
-      <c r="G9" t="s" s="10">
-        <v>51</v>
-      </c>
-      <c r="H9" t="s" s="10">
-        <v>52</v>
-      </c>
-      <c r="I9" t="s" s="10">
-        <v>53</v>
+      <c r="A9" t="s" s="6">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s" s="8">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s" s="8">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s" s="8">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s" s="8">
+        <v>62</v>
+      </c>
+      <c r="H9" t="s" s="8">
+        <v>63</v>
+      </c>
+      <c r="I9" t="s" s="8">
+        <v>64</v>
       </c>
     </row>
-    <row r="10" ht="32.05" customHeight="1">
-      <c r="A10" t="s" s="8">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="C10" t="s" s="10">
-        <v>55</v>
-      </c>
-      <c r="D10" s="11">
-        <v>6</v>
-      </c>
-      <c r="E10" s="11">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s" s="10">
-        <v>56</v>
-      </c>
-      <c r="G10" t="s" s="10">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s" s="10">
-        <v>58</v>
-      </c>
-      <c r="I10" t="s" s="10">
-        <v>59</v>
+    <row r="10" ht="44.05" customHeight="1">
+      <c r="A10" t="s" s="6">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s" s="8">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s" s="8">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s" s="8">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s" s="8">
+        <v>69</v>
+      </c>
+      <c r="H10" t="s" s="8">
+        <v>70</v>
+      </c>
+      <c r="I10" t="s" s="8">
+        <v>71</v>
       </c>
     </row>
-    <row r="11" ht="44.05" customHeight="1">
-      <c r="A11" t="s" s="8">
+    <row r="11" ht="32.05" customHeight="1">
+      <c r="A11" t="s" s="6">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s" s="8">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s" s="8">
         <v>60</v>
       </c>
-      <c r="B11" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="C11" t="s" s="10">
-        <v>61</v>
-      </c>
-      <c r="D11" s="11">
-        <v>7</v>
-      </c>
-      <c r="E11" s="11">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s" s="10">
-        <v>62</v>
-      </c>
-      <c r="G11" t="s" s="10">
-        <v>63</v>
-      </c>
-      <c r="H11" t="s" s="10">
-        <v>64</v>
-      </c>
-      <c r="I11" t="s" s="10">
-        <v>65</v>
+      <c r="F11" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s" s="8">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s" s="8">
+        <v>78</v>
       </c>
     </row>
     <row r="12" ht="32.05" customHeight="1">
-      <c r="A12" t="s" s="8">
-        <v>66</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s" s="10">
-        <v>67</v>
-      </c>
-      <c r="D12" s="11">
-        <v>8</v>
-      </c>
-      <c r="E12" s="11">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s" s="10">
-        <v>68</v>
-      </c>
-      <c r="G12" t="s" s="10">
-        <v>69</v>
-      </c>
-      <c r="H12" t="s" s="10">
-        <v>70</v>
-      </c>
-      <c r="I12" t="s" s="10">
-        <v>71</v>
+      <c r="A12" t="s" s="6">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s" s="8">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="F12" t="s" s="8">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s" s="8">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s" s="8">
+        <v>85</v>
+      </c>
+      <c r="I12" t="s" s="8">
+        <v>86</v>
       </c>
     </row>
-    <row r="13" ht="32.05" customHeight="1">
-      <c r="A13" t="s" s="8">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="C13" t="s" s="10">
+    <row r="13" ht="44.05" customHeight="1">
+      <c r="A13" t="s" s="6">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s" s="7">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s" s="8">
+        <v>88</v>
+      </c>
+      <c r="D13" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s" s="8">
         <v>74</v>
       </c>
-      <c r="D13" s="11">
-        <v>5</v>
-      </c>
-      <c r="E13" s="11">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s" s="10">
-        <v>75</v>
-      </c>
-      <c r="G13" t="s" s="10">
-        <v>76</v>
-      </c>
-      <c r="H13" t="s" s="10">
-        <v>77</v>
-      </c>
-      <c r="I13" t="s" s="10">
-        <v>78</v>
+      <c r="F13" t="s" s="8">
+        <v>89</v>
+      </c>
+      <c r="G13" t="s" s="8">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s" s="8">
+        <v>91</v>
+      </c>
+      <c r="I13" t="s" s="8">
+        <v>92</v>
       </c>
     </row>
-    <row r="14" ht="44.05" customHeight="1">
-      <c r="A14" t="s" s="8">
-        <v>79</v>
-      </c>
-      <c r="B14" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="C14" t="s" s="10">
+    <row r="14" ht="32.05" customHeight="1">
+      <c r="A14" t="s" s="6">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s" s="7">
         <v>80</v>
       </c>
-      <c r="D14" s="11">
-        <v>4</v>
-      </c>
-      <c r="E14" s="11">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s" s="10">
-        <v>81</v>
-      </c>
-      <c r="G14" t="s" s="10">
-        <v>82</v>
-      </c>
-      <c r="H14" t="s" s="10">
-        <v>83</v>
-      </c>
-      <c r="I14" t="s" s="10">
-        <v>84</v>
+      <c r="C14" t="s" s="8">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s" s="8">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s" s="8">
+        <v>95</v>
+      </c>
+      <c r="F14" t="s" s="8">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s" s="8">
+        <v>97</v>
+      </c>
+      <c r="H14" t="s" s="8">
+        <v>98</v>
+      </c>
+      <c r="I14" t="s" s="8">
+        <v>99</v>
       </c>
     </row>
     <row r="15" ht="32.05" customHeight="1">
-      <c r="A15" t="s" s="8">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s" s="10">
-        <v>86</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6</v>
-      </c>
-      <c r="E15" s="11">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s" s="10">
-        <v>87</v>
-      </c>
-      <c r="G15" t="s" s="10">
-        <v>88</v>
-      </c>
-      <c r="H15" t="s" s="10">
-        <v>89</v>
-      </c>
-      <c r="I15" t="s" s="10">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" ht="32.05" customHeight="1">
-      <c r="A16" t="s" s="8">
-        <v>91</v>
-      </c>
-      <c r="B16" t="s" s="9">
-        <v>92</v>
-      </c>
-      <c r="C16" t="s" s="10">
-        <v>93</v>
-      </c>
-      <c r="D16" s="11">
-        <v>10</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s" s="10">
-        <v>94</v>
-      </c>
-      <c r="G16" t="s" s="10">
+      <c r="A15" t="s" s="6">
+        <v>100</v>
+      </c>
+      <c r="B15" t="s" s="7">
+        <v>101</v>
+      </c>
+      <c r="C15" t="s" s="8">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="E15" t="s" s="8">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s" s="8">
+        <v>104</v>
+      </c>
+      <c r="G15" t="s" s="8">
+        <v>105</v>
+      </c>
+      <c r="H15" t="s" s="8">
         <v>95</v>
       </c>
-      <c r="H16" t="s" s="10">
-        <v>96</v>
-      </c>
-      <c r="I16" t="s" s="10">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="8">
-        <v>98</v>
-      </c>
-      <c r="B17" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s" s="10">
-        <v>24</v>
-      </c>
-      <c r="D17" s="11">
-        <v>1</v>
-      </c>
-      <c r="E17" s="11">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s" s="10">
-        <v>99</v>
-      </c>
-      <c r="G17" t="s" s="10">
-        <v>100</v>
-      </c>
-      <c r="H17" s="12">
-        <v>99</v>
-      </c>
-      <c r="I17" t="s" s="10">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="8">
-        <v>101</v>
-      </c>
-      <c r="B18" t="s" s="9">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s" s="10">
-        <v>102</v>
-      </c>
-      <c r="D18" s="12">
-        <v>10</v>
-      </c>
-      <c r="E18" s="12">
-        <v>2</v>
-      </c>
-      <c r="F18" t="s" s="10">
-        <v>103</v>
-      </c>
-      <c r="G18" t="s" s="10">
-        <v>104</v>
-      </c>
-      <c r="H18" s="12">
-        <v>99</v>
-      </c>
-      <c r="I18" t="s" s="10">
-        <v>105</v>
+      <c r="I15" t="s" s="8">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>